<commit_message>
Correct data where rankings were wrong way around in one is high column
</commit_message>
<xml_diff>
--- a/data/Metadata - Shiny.xlsx
+++ b/data/Metadata - Shiny.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://impservihub.sharepoint.com/sites/tpi-benchmarking/Shared Documents/MASTER DATA/Shiny Tool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\OneDrive - IS\LGBF-Spotfire\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2869,8 +2869,8 @@
   <dimension ref="A1:IN499"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E194" sqref="E191:E194"/>
+      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K186" sqref="K186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="I177"/>
       <c r="K177" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L177" s="39" t="s">
         <v>386</v>
@@ -8952,7 +8952,7 @@
       </c>
       <c r="I178"/>
       <c r="K178" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L178" s="39" t="s">
         <v>388</v>
@@ -9014,7 +9014,7 @@
       </c>
       <c r="I180"/>
       <c r="K180" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L180" s="39" t="s">
         <v>392</v>
@@ -9108,7 +9108,7 @@
       </c>
       <c r="I183"/>
       <c r="K183" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L183" t="str">
         <f t="shared" ref="L183:L186" si="3">A183</f>
@@ -9140,7 +9140,7 @@
       </c>
       <c r="I184"/>
       <c r="K184" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="L184" t="str">
         <f t="shared" si="3"/>
@@ -9172,7 +9172,7 @@
       </c>
       <c r="I185"/>
       <c r="K185" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L185" t="str">
         <f t="shared" si="3"/>
@@ -9204,7 +9204,7 @@
       </c>
       <c r="I186"/>
       <c r="K186" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="L186" t="str">
         <f t="shared" si="3"/>
@@ -12660,18 +12660,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12878,26 +12878,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
+    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed ranks for last page;  Add ECON6 Real values in metadata; Sort SW1 names so that cash values do not appear when real is selected in page 3
</commit_message>
<xml_diff>
--- a/data/Metadata - Shiny.xlsx
+++ b/data/Metadata - Shiny.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\OneDrive - IS\LGBF-Spotfire\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="6_{B20E5C06-F44C-4DAE-9511-A46F5BA94FCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10770"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$L$121</definedName>
     <definedName name="_ftnref1" localSheetId="0">metadata!$I$110</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="409">
   <si>
     <t>Variable name</t>
   </si>
@@ -641,9 +642,6 @@
     <t>The cost per dwelling of collecting Council Tax adjusted for inflation</t>
   </si>
   <si>
-    <t>Older Persons (over 65's)  Home Care Costs per Hour adjusted for inflation</t>
-  </si>
-  <si>
     <t>Older persons (over 65's) Residential Care Costs per week per resident adjusted for inflation</t>
   </si>
   <si>
@@ -1257,12 +1255,21 @@
   </si>
   <si>
     <t>Immediately available employment land as a % of total land allocated for employment purposes in the local development plan</t>
+  </si>
+  <si>
+    <t>ECON6-Real</t>
+  </si>
+  <si>
+    <t>Cost of tourism and economic development per 1,000 population adjusted for inflation</t>
+  </si>
+  <si>
+    <t>Older Persons (Over 65's) Home Care Costs per Hour adjusted for inflation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
@@ -2862,15 +2869,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:IN499"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K186" sqref="K186"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3164,7 +3171,7 @@
     </row>
     <row r="2" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -3197,7 +3204,7 @@
     </row>
     <row r="3" spans="1:248" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
@@ -3229,7 +3236,7 @@
     </row>
     <row r="4" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>21</v>
@@ -3262,7 +3269,7 @@
     </row>
     <row r="5" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
@@ -3297,7 +3304,7 @@
     </row>
     <row r="6" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>30</v>
@@ -3431,7 +3438,7 @@
         <v>No of Pupils Secondary</v>
       </c>
       <c r="M9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:248" ht="24" x14ac:dyDescent="0.2">
@@ -3537,7 +3544,7 @@
     </row>
     <row r="13" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>42</v>
@@ -3570,7 +3577,7 @@
     </row>
     <row r="14" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>43</v>
@@ -3603,7 +3610,7 @@
     </row>
     <row r="15" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>44</v>
@@ -3636,7 +3643,7 @@
     </row>
     <row r="16" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>45</v>
@@ -3871,7 +3878,7 @@
     </row>
     <row r="23" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>56</v>
@@ -3904,7 +3911,7 @@
     </row>
     <row r="24" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>57</v>
@@ -4139,7 +4146,7 @@
     </row>
     <row r="31" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>71</v>
@@ -4172,7 +4179,7 @@
     </row>
     <row r="32" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>72</v>
@@ -4205,7 +4212,7 @@
     </row>
     <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>73</v>
@@ -4238,7 +4245,7 @@
     </row>
     <row r="34" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>74</v>
@@ -4271,7 +4278,7 @@
     </row>
     <row r="35" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>75</v>
@@ -4304,7 +4311,7 @@
     </row>
     <row r="36" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>76</v>
@@ -4337,7 +4344,7 @@
     </row>
     <row r="37" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>77</v>
@@ -4370,7 +4377,7 @@
     </row>
     <row r="38" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>78</v>
@@ -4403,7 +4410,7 @@
     </row>
     <row r="39" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>79</v>
@@ -4436,7 +4443,7 @@
     </row>
     <row r="40" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>80</v>
@@ -4469,7 +4476,7 @@
     </row>
     <row r="41" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>81</v>
@@ -4706,7 +4713,7 @@
     </row>
     <row r="48" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>95</v>
@@ -4772,7 +4779,7 @@
     </row>
     <row r="50" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>99</v>
@@ -4976,7 +4983,7 @@
     </row>
     <row r="56" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>111</v>
@@ -4998,7 +5005,7 @@
         <v>17</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>112</v>
@@ -5078,7 +5085,7 @@
     </row>
     <row r="59" spans="1:12" ht="72.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>116</v>
@@ -5384,7 +5391,7 @@
     </row>
     <row r="68" spans="1:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>132</v>
@@ -5519,7 +5526,7 @@
     </row>
     <row r="72" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>138</v>
@@ -5552,7 +5559,7 @@
     </row>
     <row r="73" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>140</v>
@@ -5585,7 +5592,7 @@
     </row>
     <row r="74" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>141</v>
@@ -5651,7 +5658,7 @@
     </row>
     <row r="76" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>143</v>
@@ -5686,7 +5693,7 @@
     </row>
     <row r="77" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>146</v>
@@ -5719,7 +5726,7 @@
     </row>
     <row r="78" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>147</v>
@@ -5752,7 +5759,7 @@
     </row>
     <row r="79" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>149</v>
@@ -5785,7 +5792,7 @@
     </row>
     <row r="80" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>150</v>
@@ -5818,7 +5825,7 @@
     </row>
     <row r="81" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>151</v>
@@ -5851,7 +5858,7 @@
     </row>
     <row r="82" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>152</v>
@@ -5884,7 +5891,7 @@
     </row>
     <row r="83" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>153</v>
@@ -5917,7 +5924,7 @@
     </row>
     <row r="84" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B84" s="31" t="s">
         <v>154</v>
@@ -5950,7 +5957,7 @@
     </row>
     <row r="85" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>155</v>
@@ -5983,7 +5990,7 @@
     </row>
     <row r="86" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B86" s="33" t="s">
         <v>156</v>
@@ -6016,7 +6023,7 @@
     </row>
     <row r="87" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>157</v>
@@ -6046,7 +6053,7 @@
     </row>
     <row r="88" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B88" s="33" t="s">
         <v>158</v>
@@ -6077,7 +6084,7 @@
     </row>
     <row r="89" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>159</v>
@@ -6110,7 +6117,7 @@
     </row>
     <row r="90" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>160</v>
@@ -6143,7 +6150,7 @@
     </row>
     <row r="91" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>161</v>
@@ -6207,7 +6214,7 @@
     </row>
     <row r="93" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B93" s="33" t="s">
         <v>163</v>
@@ -6271,7 +6278,7 @@
     </row>
     <row r="95" spans="1:12" s="34" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B95" s="31" t="s">
         <v>165</v>
@@ -6333,7 +6340,7 @@
     </row>
     <row r="97" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>167</v>
@@ -6364,7 +6371,7 @@
     </row>
     <row r="98" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B98" s="33" t="s">
         <v>168</v>
@@ -6397,7 +6404,7 @@
     </row>
     <row r="99" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B99" s="36" t="s">
         <v>169</v>
@@ -6496,7 +6503,7 @@
     </row>
     <row r="102" spans="1:12" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B102" s="32" t="s">
         <v>176</v>
@@ -6529,7 +6536,7 @@
     </row>
     <row r="103" spans="1:12" s="34" customFormat="1" ht="276" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B103" s="32" t="s">
         <v>181</v>
@@ -6562,7 +6569,7 @@
     </row>
     <row r="104" spans="1:12" s="34" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B104" s="32" t="s">
         <v>184</v>
@@ -6595,7 +6602,7 @@
     </row>
     <row r="105" spans="1:12" s="34" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B105" s="32" t="s">
         <v>186</v>
@@ -6628,7 +6635,7 @@
     </row>
     <row r="106" spans="1:12" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B106" s="32" t="s">
         <v>187</v>
@@ -6661,7 +6668,7 @@
     </row>
     <row r="107" spans="1:12" s="34" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B107" s="32" t="s">
         <v>189</v>
@@ -6694,7 +6701,7 @@
     </row>
     <row r="108" spans="1:12" s="34" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B108" s="32" t="s">
         <v>191</v>
@@ -6725,7 +6732,7 @@
     </row>
     <row r="109" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B109" s="32" t="s">
         <v>192</v>
@@ -6756,7 +6763,7 @@
     </row>
     <row r="110" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>193</v>
@@ -6787,7 +6794,7 @@
     </row>
     <row r="111" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>194</v>
@@ -6820,7 +6827,7 @@
     </row>
     <row r="112" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>195</v>
@@ -6853,7 +6860,7 @@
     </row>
     <row r="113" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>196</v>
@@ -6886,7 +6893,7 @@
     </row>
     <row r="114" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>197</v>
@@ -6919,7 +6926,7 @@
     </row>
     <row r="115" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>198</v>
@@ -6952,7 +6959,7 @@
     </row>
     <row r="116" spans="1:12" s="34" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>199</v>
@@ -6985,7 +6992,7 @@
     </row>
     <row r="117" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>200</v>
@@ -7018,10 +7025,10 @@
     </row>
     <row r="118" spans="1:12" s="34" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B118" s="33" t="s">
-        <v>201</v>
+        <v>408</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>22</v>
@@ -7051,10 +7058,10 @@
     </row>
     <row r="119" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B119" s="38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C119" s="9" t="s">
         <v>22</v>
@@ -7083,10 +7090,10 @@
     </row>
     <row r="120" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C120" s="9" t="s">
         <v>59</v>
@@ -7115,10 +7122,10 @@
     </row>
     <row r="121" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C121" s="9" t="s">
         <v>59</v>
@@ -7147,10 +7154,10 @@
     </row>
     <row r="122" spans="1:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C122" s="9" t="s">
         <v>59</v>
@@ -7179,10 +7186,10 @@
     </row>
     <row r="123" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B123" s="38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>59</v>
@@ -7211,10 +7218,10 @@
     </row>
     <row r="124" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C124" s="9" t="s">
         <v>59</v>
@@ -7243,10 +7250,10 @@
     </row>
     <row r="125" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C125" s="9" t="s">
         <v>59</v>
@@ -7275,10 +7282,10 @@
     </row>
     <row r="126" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C126" s="9" t="s">
         <v>59</v>
@@ -7307,10 +7314,10 @@
     </row>
     <row r="127" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B127" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C127" s="9" t="s">
         <v>59</v>
@@ -7339,10 +7346,10 @@
     </row>
     <row r="128" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B128" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C128" s="9" t="s">
         <v>59</v>
@@ -7372,10 +7379,10 @@
     </row>
     <row r="129" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B129" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C129" s="9" t="s">
         <v>22</v>
@@ -7405,10 +7412,10 @@
     </row>
     <row r="130" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>22</v>
@@ -7438,10 +7445,10 @@
     </row>
     <row r="131" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C131" s="9" t="s">
         <v>59</v>
@@ -7471,10 +7478,10 @@
     </row>
     <row r="132" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C132" s="9" t="s">
         <v>59</v>
@@ -7504,10 +7511,10 @@
     </row>
     <row r="133" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C133" s="9" t="s">
         <v>59</v>
@@ -7537,10 +7544,10 @@
     </row>
     <row r="134" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C134" s="9" t="s">
         <v>59</v>
@@ -7570,10 +7577,10 @@
     </row>
     <row r="135" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C135" s="9" t="s">
         <v>59</v>
@@ -7603,10 +7610,10 @@
     </row>
     <row r="136" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B136" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>59</v>
@@ -7636,10 +7643,10 @@
     </row>
     <row r="137" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B137" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>22</v>
@@ -7669,10 +7676,10 @@
     </row>
     <row r="138" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>22</v>
@@ -7702,10 +7709,10 @@
     </row>
     <row r="139" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>59</v>
@@ -7735,10 +7742,10 @@
     </row>
     <row r="140" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B140" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>59</v>
@@ -7768,10 +7775,10 @@
     </row>
     <row r="141" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B141" s="33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>59</v>
@@ -7801,10 +7808,10 @@
     </row>
     <row r="142" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C142" t="s">
         <v>59</v>
@@ -7833,10 +7840,10 @@
     </row>
     <row r="143" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>59</v>
@@ -7866,10 +7873,10 @@
     </row>
     <row r="144" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C144" s="36" t="s">
         <v>59</v>
@@ -7899,10 +7906,10 @@
     </row>
     <row r="145" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C145" s="36" t="s">
         <v>59</v>
@@ -7929,10 +7936,10 @@
     </row>
     <row r="146" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C146" s="36" t="s">
         <v>59</v>
@@ -7959,10 +7966,10 @@
     </row>
     <row r="147" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C147" s="36" t="s">
         <v>59</v>
@@ -7992,10 +7999,10 @@
     </row>
     <row r="148" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C148" s="36" t="s">
         <v>59</v>
@@ -8025,10 +8032,10 @@
     </row>
     <row r="149" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C149" s="36" t="s">
         <v>59</v>
@@ -8058,10 +8065,10 @@
     </row>
     <row r="150" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C150" s="36" t="s">
         <v>59</v>
@@ -8088,10 +8095,10 @@
     </row>
     <row r="151" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C151" s="36" t="s">
         <v>59</v>
@@ -8118,10 +8125,10 @@
     </row>
     <row r="152" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B152" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="C152" s="36" t="s">
         <v>22</v>
@@ -8144,15 +8151,15 @@
         <v>26</v>
       </c>
       <c r="L152" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="153" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="C153" t="s">
         <v>22</v>
@@ -8175,15 +8182,15 @@
         <v>26</v>
       </c>
       <c r="L153" s="34" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B154" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="C154" t="s">
         <v>22</v>
@@ -8206,15 +8213,15 @@
         <v>26</v>
       </c>
       <c r="L154" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B155" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="C155" t="s">
         <v>22</v>
@@ -8237,15 +8244,15 @@
         <v>26</v>
       </c>
       <c r="L155" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B156" s="32" t="s">
         <v>243</v>
-      </c>
-      <c r="B156" s="32" t="s">
-        <v>244</v>
       </c>
       <c r="C156" s="32" t="s">
         <v>22</v>
@@ -8269,15 +8276,15 @@
         <v>26</v>
       </c>
       <c r="L156" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B157" s="32" t="s">
         <v>245</v>
-      </c>
-      <c r="B157" s="32" t="s">
-        <v>246</v>
       </c>
       <c r="C157" s="32" t="s">
         <v>22</v>
@@ -8301,15 +8308,15 @@
         <v>26</v>
       </c>
       <c r="L157" s="34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B158" s="32" t="s">
         <v>247</v>
-      </c>
-      <c r="B158" s="32" t="s">
-        <v>248</v>
       </c>
       <c r="C158" s="32" t="s">
         <v>22</v>
@@ -8333,15 +8340,15 @@
         <v>26</v>
       </c>
       <c r="L158" s="34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B159" s="32" t="s">
         <v>249</v>
-      </c>
-      <c r="B159" s="32" t="s">
-        <v>250</v>
       </c>
       <c r="C159" s="32" t="s">
         <v>22</v>
@@ -8365,15 +8372,15 @@
         <v>26</v>
       </c>
       <c r="L159" s="34" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B160" s="32" t="s">
         <v>251</v>
-      </c>
-      <c r="B160" s="32" t="s">
-        <v>252</v>
       </c>
       <c r="C160" s="32" t="s">
         <v>22</v>
@@ -8397,15 +8404,15 @@
         <v>26</v>
       </c>
       <c r="L160" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="161" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A161" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="C161" t="s">
         <v>22</v>
@@ -8428,15 +8435,15 @@
         <v>26</v>
       </c>
       <c r="L161" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A162" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="B162" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C162" t="s">
         <v>22</v>
@@ -8459,15 +8466,15 @@
         <v>26</v>
       </c>
       <c r="L162" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A163" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="B163" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="C163" t="s">
         <v>22</v>
@@ -8490,15 +8497,15 @@
         <v>26</v>
       </c>
       <c r="L163" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A164" s="39" t="s">
+        <v>258</v>
+      </c>
+      <c r="B164" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="C164" t="s">
         <v>22</v>
@@ -8521,15 +8528,15 @@
         <v>26</v>
       </c>
       <c r="L164" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A165" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="C165" t="s">
         <v>22</v>
@@ -8552,15 +8559,15 @@
         <v>26</v>
       </c>
       <c r="L165" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A166" s="39" t="s">
+        <v>262</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="C166" t="s">
         <v>22</v>
@@ -8583,15 +8590,15 @@
         <v>26</v>
       </c>
       <c r="L166" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A167" s="39" t="s">
+        <v>264</v>
+      </c>
+      <c r="B167" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="C167" t="s">
         <v>22</v>
@@ -8614,15 +8621,15 @@
         <v>26</v>
       </c>
       <c r="L167" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A168" s="39" t="s">
+        <v>266</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="C168" t="s">
         <v>22</v>
@@ -8645,15 +8652,15 @@
         <v>26</v>
       </c>
       <c r="L168" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A169" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="C169" t="s">
         <v>22</v>
@@ -8676,15 +8683,15 @@
         <v>26</v>
       </c>
       <c r="L169" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A170" s="39" t="s">
+        <v>270</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="C170" t="s">
         <v>22</v>
@@ -8707,15 +8714,15 @@
         <v>26</v>
       </c>
       <c r="L170" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A171" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="C171" t="s">
         <v>22</v>
@@ -8738,15 +8745,15 @@
         <v>26</v>
       </c>
       <c r="L171" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A172" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="C172" t="s">
         <v>59</v>
@@ -8769,15 +8776,15 @@
         <v>17</v>
       </c>
       <c r="L172" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A173" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>379</v>
       </c>
       <c r="C173" t="s">
         <v>22</v>
@@ -8800,15 +8807,15 @@
         <v>26</v>
       </c>
       <c r="L173" s="39" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A174" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="B174" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="C174" t="s">
         <v>22</v>
@@ -8831,15 +8838,15 @@
         <v>26</v>
       </c>
       <c r="L174" s="39" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A175" s="39" t="s">
+        <v>381</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="C175" t="s">
         <v>22</v>
@@ -8862,15 +8869,15 @@
         <v>26</v>
       </c>
       <c r="L175" s="39" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="176" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A176" s="39" t="s">
+        <v>383</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="C176" t="s">
         <v>22</v>
@@ -8893,15 +8900,15 @@
         <v>26</v>
       </c>
       <c r="L176" s="39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A177" s="39" t="s">
+        <v>385</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="C177" t="s">
         <v>22</v>
@@ -8924,15 +8931,15 @@
         <v>17</v>
       </c>
       <c r="L177" s="39" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A178" s="39" t="s">
+        <v>387</v>
+      </c>
+      <c r="B178" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>389</v>
       </c>
       <c r="C178" t="s">
         <v>22</v>
@@ -8955,15 +8962,15 @@
         <v>17</v>
       </c>
       <c r="L178" s="39" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A179" s="39" t="s">
+        <v>389</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C179" t="s">
         <v>22</v>
@@ -8986,15 +8993,15 @@
         <v>26</v>
       </c>
       <c r="L179" s="39" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A180" s="39" t="s">
+        <v>391</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="C180" t="s">
         <v>22</v>
@@ -9017,15 +9024,15 @@
         <v>17</v>
       </c>
       <c r="L180" s="39" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A181" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="C181" t="s">
         <v>22</v>
@@ -9048,15 +9055,15 @@
         <v>17</v>
       </c>
       <c r="L181" s="39" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A182" s="39" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C182" t="s">
         <v>59</v>
@@ -9085,10 +9092,10 @@
     </row>
     <row r="183" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A183" s="39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C183" t="s">
         <v>59</v>
@@ -9117,10 +9124,10 @@
     </row>
     <row r="184" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A184" s="39" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C184" t="s">
         <v>59</v>
@@ -9149,10 +9156,10 @@
     </row>
     <row r="185" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A185" s="39" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C185" t="s">
         <v>59</v>
@@ -9181,10 +9188,10 @@
     </row>
     <row r="186" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A186" s="39" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C186" t="s">
         <v>59</v>
@@ -9211,15 +9218,36 @@
         <v>ECON10</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A187" s="39"/>
-      <c r="C187"/>
-      <c r="D187"/>
+    <row r="187" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+      <c r="A187" s="39" t="s">
+        <v>406</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C187" t="s">
+        <v>59</v>
+      </c>
+      <c r="D187" t="s">
+        <v>170</v>
+      </c>
       <c r="E187"/>
-      <c r="F187"/>
-      <c r="G187"/>
-      <c r="H187"/>
+      <c r="F187" t="s">
+        <v>24</v>
+      </c>
+      <c r="G187" t="s">
+        <v>28</v>
+      </c>
+      <c r="H187" t="s">
+        <v>26</v>
+      </c>
       <c r="I187"/>
+      <c r="K187" t="s">
+        <v>17</v>
+      </c>
+      <c r="L187" s="39" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" s="39"/>
@@ -12347,7 +12375,7 @@
       <formula>LEN(TRIM(M1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A187:IO1048576 A182:E186 I182:IO186">
+  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A182:E186 I182:IO186 A187:IO1048576">
     <cfRule type="notContainsBlanks" dxfId="63" priority="64">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
@@ -12650,7 +12678,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Wrong values" error="The cell accepts only Yes/No values." sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Wrong values" error="The cell accepts only Yes/No values." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12888,15 +12916,15 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
     <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
-    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Change ranking for financial sustainability
</commit_message>
<xml_diff>
--- a/data/Metadata - Shiny.xlsx
+++ b/data/Metadata - Shiny.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\OneDrive - IS\LGBF-Spotfire\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{B20E5C06-F44C-4DAE-9511-A46F5BA94FCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C92578-C1B8-4CDD-89B5-AC348BD92276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$L$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$M$197</definedName>
     <definedName name="_ftnref1" localSheetId="0">metadata!$I$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="445">
   <si>
     <t>Variable name</t>
   </si>
@@ -792,15 +792,9 @@
     <t>CHN13a</t>
   </si>
   <si>
-    <t>Percentage of pupils achieving expected levels in Reading P1</t>
-  </si>
-  <si>
     <t>CHN13b</t>
   </si>
   <si>
-    <t>Percentage of pupils achieving expected levels in Reading P3</t>
-  </si>
-  <si>
     <t>CHN13c</t>
   </si>
   <si>
@@ -810,15 +804,9 @@
     <t>CHN14a</t>
   </si>
   <si>
-    <t>Percentage of pupils achieving expected levels in Writing P1</t>
-  </si>
-  <si>
     <t>CHN14b</t>
   </si>
   <si>
-    <t>Percentage of pupils achieving expected levels in Writing P3</t>
-  </si>
-  <si>
     <t>CHN14c</t>
   </si>
   <si>
@@ -1264,13 +1252,133 @@
   </si>
   <si>
     <t>Older Persons (Over 65's) Home Care Costs per Hour adjusted for inflation</t>
+  </si>
+  <si>
+    <t>SW4c</t>
+  </si>
+  <si>
+    <t>SW4d</t>
+  </si>
+  <si>
+    <t>SW4e</t>
+  </si>
+  <si>
+    <t>SW6</t>
+  </si>
+  <si>
+    <t>SW7</t>
+  </si>
+  <si>
+    <t>SW8</t>
+  </si>
+  <si>
+    <t>Percentage of adults supported at home who agree that they are supported to live as independently as possible</t>
+  </si>
+  <si>
+    <t>Percentage of adults supported at home who agree that they had a say in how their help, care or support was provided</t>
+  </si>
+  <si>
+    <t>Percentage of carers who feel supported to continue in their caring role</t>
+  </si>
+  <si>
+    <t>Proportion of care services graded 'good' (4) or better in Care Inspectorate inspections</t>
+  </si>
+  <si>
+    <t>Rate of readmission to hospital within 28 days per 1,000 discharges</t>
+  </si>
+  <si>
+    <t>Number of readmissions to an acute hospital within 28 days of discharge</t>
+  </si>
+  <si>
+    <t>Number of discharges</t>
+  </si>
+  <si>
+    <t>Number of days people spend in hospital when they are ready to be discharged, per 1,000 population (75+)</t>
+  </si>
+  <si>
+    <t>Number of bed days people spend in hospital when they are ready to be discharged</t>
+  </si>
+  <si>
+    <t>MYE Population (75+)</t>
+  </si>
+  <si>
+    <t>Percentage of  P1, P4 and P7 pupils combined achieving expected CFE Level in Literacy</t>
+  </si>
+  <si>
+    <t>Percentage of  P1, P4 and P7 pupils combined achieving expected CFE Level in Numeracy</t>
+  </si>
+  <si>
+    <t>Literacy Attainment Gap (P1,4,7 Combined) - percentage point gap between the least deprived and most deprived pupils</t>
+  </si>
+  <si>
+    <t>Numeracy Attainment Gap (P1,4,7 Combined) - percentage point gap between the least deprived and most deprived pupils</t>
+  </si>
+  <si>
+    <t>HSN5a</t>
+  </si>
+  <si>
+    <t>% of council dwellings that are energy efficient</t>
+  </si>
+  <si>
+    <t>CLIM1</t>
+  </si>
+  <si>
+    <t>CLIM2</t>
+  </si>
+  <si>
+    <t>CO2 emissions area wide per capita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2 emissions area wide: emissions within scope of LA per capita </t>
+  </si>
+  <si>
+    <t>Tackling Climate Change</t>
+  </si>
+  <si>
+    <t>FINSUS1</t>
+  </si>
+  <si>
+    <t>FINSUS2</t>
+  </si>
+  <si>
+    <t>FINSUS3</t>
+  </si>
+  <si>
+    <t>FINSUS4</t>
+  </si>
+  <si>
+    <t>FINSUS5</t>
+  </si>
+  <si>
+    <t>Total useable reserves as a % of council annual budgeted revenue</t>
+  </si>
+  <si>
+    <t>Uncommitted General Fund Balance as a % of council annual budgeted net revenue</t>
+  </si>
+  <si>
+    <t>Ratio of Financing Costs to Net Revenue Stream - General Fund</t>
+  </si>
+  <si>
+    <t>Ratio of Financing Costs to Net Revenue Stream - Housing Revenue Account</t>
+  </si>
+  <si>
+    <t>Actual outturn as a percentage of budgeted expenditure</t>
+  </si>
+  <si>
+    <t>Financial Sustainability</t>
+  </si>
+  <si>
+    <t>Net outrun revenue expenditure as reported to committee (£000s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net budgeted revenue expenditure as reported to committee (£000s) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
@@ -1287,16 +1395,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1432,13 +1556,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1565,11 +1698,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="65">
+  <dxfs count="66">
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2873,11 +3030,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:IN499"/>
+  <dimension ref="A1:IN501"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
+      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K205" sqref="K205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3171,7 +3328,7 @@
     </row>
     <row r="2" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -3204,7 +3361,7 @@
     </row>
     <row r="3" spans="1:248" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
@@ -3236,7 +3393,7 @@
     </row>
     <row r="4" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>21</v>
@@ -3269,7 +3426,7 @@
     </row>
     <row r="5" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>27</v>
@@ -3304,7 +3461,7 @@
     </row>
     <row r="6" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>30</v>
@@ -3438,7 +3595,7 @@
         <v>No of Pupils Secondary</v>
       </c>
       <c r="M9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:248" ht="24" x14ac:dyDescent="0.2">
@@ -3544,7 +3701,7 @@
     </row>
     <row r="13" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>42</v>
@@ -3577,7 +3734,7 @@
     </row>
     <row r="14" spans="1:248" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>43</v>
@@ -3610,7 +3767,7 @@
     </row>
     <row r="15" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>44</v>
@@ -3643,7 +3800,7 @@
     </row>
     <row r="16" spans="1:248" ht="36" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>45</v>
@@ -3878,7 +4035,7 @@
     </row>
     <row r="23" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>56</v>
@@ -3911,7 +4068,7 @@
     </row>
     <row r="24" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>57</v>
@@ -4146,7 +4303,7 @@
     </row>
     <row r="31" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>71</v>
@@ -4179,7 +4336,7 @@
     </row>
     <row r="32" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>72</v>
@@ -4212,7 +4369,7 @@
     </row>
     <row r="33" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>73</v>
@@ -4245,7 +4402,7 @@
     </row>
     <row r="34" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>74</v>
@@ -4278,7 +4435,7 @@
     </row>
     <row r="35" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>75</v>
@@ -4311,7 +4468,7 @@
     </row>
     <row r="36" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>76</v>
@@ -4344,7 +4501,7 @@
     </row>
     <row r="37" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>77</v>
@@ -4377,7 +4534,7 @@
     </row>
     <row r="38" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>78</v>
@@ -4410,7 +4567,7 @@
     </row>
     <row r="39" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>79</v>
@@ -4443,7 +4600,7 @@
     </row>
     <row r="40" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>80</v>
@@ -4476,7 +4633,7 @@
     </row>
     <row r="41" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>81</v>
@@ -4713,7 +4870,7 @@
     </row>
     <row r="48" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B48" s="23" t="s">
         <v>95</v>
@@ -4779,7 +4936,7 @@
     </row>
     <row r="50" spans="1:12" ht="84" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>99</v>
@@ -4983,7 +5140,7 @@
     </row>
     <row r="56" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>111</v>
@@ -5005,7 +5162,7 @@
         <v>17</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>112</v>
@@ -5085,7 +5242,7 @@
     </row>
     <row r="59" spans="1:12" ht="72.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>116</v>
@@ -5391,7 +5548,7 @@
     </row>
     <row r="68" spans="1:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>132</v>
@@ -5526,7 +5683,7 @@
     </row>
     <row r="72" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>138</v>
@@ -5559,7 +5716,7 @@
     </row>
     <row r="73" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>140</v>
@@ -5592,7 +5749,7 @@
     </row>
     <row r="74" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B74" s="19" t="s">
         <v>141</v>
@@ -5658,7 +5815,7 @@
     </row>
     <row r="76" spans="1:12" ht="72" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>143</v>
@@ -5693,7 +5850,7 @@
     </row>
     <row r="77" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>146</v>
@@ -5726,7 +5883,7 @@
     </row>
     <row r="78" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>147</v>
@@ -5759,7 +5916,7 @@
     </row>
     <row r="79" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>149</v>
@@ -5792,7 +5949,7 @@
     </row>
     <row r="80" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>150</v>
@@ -5825,7 +5982,7 @@
     </row>
     <row r="81" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>151</v>
@@ -5858,7 +6015,7 @@
     </row>
     <row r="82" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>152</v>
@@ -5891,7 +6048,7 @@
     </row>
     <row r="83" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B83" s="19" t="s">
         <v>153</v>
@@ -5924,7 +6081,7 @@
     </row>
     <row r="84" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B84" s="31" t="s">
         <v>154</v>
@@ -5957,7 +6114,7 @@
     </row>
     <row r="85" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>155</v>
@@ -5990,7 +6147,7 @@
     </row>
     <row r="86" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B86" s="33" t="s">
         <v>156</v>
@@ -6023,7 +6180,7 @@
     </row>
     <row r="87" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>157</v>
@@ -6053,7 +6210,7 @@
     </row>
     <row r="88" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B88" s="33" t="s">
         <v>158</v>
@@ -6084,7 +6241,7 @@
     </row>
     <row r="89" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>159</v>
@@ -6117,7 +6274,7 @@
     </row>
     <row r="90" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>160</v>
@@ -6150,7 +6307,7 @@
     </row>
     <row r="91" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>161</v>
@@ -6214,7 +6371,7 @@
     </row>
     <row r="93" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B93" s="33" t="s">
         <v>163</v>
@@ -6278,7 +6435,7 @@
     </row>
     <row r="95" spans="1:12" s="34" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B95" s="31" t="s">
         <v>165</v>
@@ -6340,7 +6497,7 @@
     </row>
     <row r="97" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>167</v>
@@ -6371,7 +6528,7 @@
     </row>
     <row r="98" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B98" s="33" t="s">
         <v>168</v>
@@ -6404,7 +6561,7 @@
     </row>
     <row r="99" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B99" s="36" t="s">
         <v>169</v>
@@ -6503,7 +6660,7 @@
     </row>
     <row r="102" spans="1:12" s="34" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B102" s="32" t="s">
         <v>176</v>
@@ -6536,7 +6693,7 @@
     </row>
     <row r="103" spans="1:12" s="34" customFormat="1" ht="276" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B103" s="32" t="s">
         <v>181</v>
@@ -6569,7 +6726,7 @@
     </row>
     <row r="104" spans="1:12" s="34" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B104" s="32" t="s">
         <v>184</v>
@@ -6602,7 +6759,7 @@
     </row>
     <row r="105" spans="1:12" s="34" customFormat="1" ht="240" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B105" s="32" t="s">
         <v>186</v>
@@ -6635,7 +6792,7 @@
     </row>
     <row r="106" spans="1:12" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B106" s="32" t="s">
         <v>187</v>
@@ -6668,7 +6825,7 @@
     </row>
     <row r="107" spans="1:12" s="34" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B107" s="32" t="s">
         <v>189</v>
@@ -6701,7 +6858,7 @@
     </row>
     <row r="108" spans="1:12" s="34" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B108" s="32" t="s">
         <v>191</v>
@@ -6732,7 +6889,7 @@
     </row>
     <row r="109" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B109" s="32" t="s">
         <v>192</v>
@@ -6763,7 +6920,7 @@
     </row>
     <row r="110" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>193</v>
@@ -6794,7 +6951,7 @@
     </row>
     <row r="111" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>194</v>
@@ -6827,7 +6984,7 @@
     </row>
     <row r="112" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>195</v>
@@ -6860,7 +7017,7 @@
     </row>
     <row r="113" spans="1:12" s="34" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>196</v>
@@ -6893,7 +7050,7 @@
     </row>
     <row r="114" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>197</v>
@@ -6926,7 +7083,7 @@
     </row>
     <row r="115" spans="1:12" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>198</v>
@@ -6959,7 +7116,7 @@
     </row>
     <row r="116" spans="1:12" s="34" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>199</v>
@@ -6992,7 +7149,7 @@
     </row>
     <row r="117" spans="1:12" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>200</v>
@@ -7025,10 +7182,10 @@
     </row>
     <row r="118" spans="1:12" s="34" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B118" s="33" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>22</v>
@@ -7058,7 +7215,7 @@
     </row>
     <row r="119" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B119" s="38" t="s">
         <v>201</v>
@@ -7090,7 +7247,7 @@
     </row>
     <row r="120" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>202</v>
@@ -7122,7 +7279,7 @@
     </row>
     <row r="121" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>203</v>
@@ -7154,7 +7311,7 @@
     </row>
     <row r="122" spans="1:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>204</v>
@@ -7186,7 +7343,7 @@
     </row>
     <row r="123" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B123" s="38" t="s">
         <v>205</v>
@@ -7218,7 +7375,7 @@
     </row>
     <row r="124" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B124" s="19" t="s">
         <v>206</v>
@@ -7250,7 +7407,7 @@
     </row>
     <row r="125" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B125" s="19" t="s">
         <v>207</v>
@@ -7282,7 +7439,7 @@
     </row>
     <row r="126" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B126" s="19" t="s">
         <v>208</v>
@@ -7314,7 +7471,7 @@
     </row>
     <row r="127" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B127" s="19" t="s">
         <v>209</v>
@@ -7346,7 +7503,7 @@
     </row>
     <row r="128" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B128" s="19" t="s">
         <v>210</v>
@@ -7379,7 +7536,7 @@
     </row>
     <row r="129" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B129" s="19" t="s">
         <v>211</v>
@@ -7412,7 +7569,7 @@
     </row>
     <row r="130" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B130" s="19" t="s">
         <v>212</v>
@@ -7445,7 +7602,7 @@
     </row>
     <row r="131" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B131" s="19" t="s">
         <v>213</v>
@@ -7478,7 +7635,7 @@
     </row>
     <row r="132" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B132" s="19" t="s">
         <v>214</v>
@@ -7511,7 +7668,7 @@
     </row>
     <row r="133" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B133" s="19" t="s">
         <v>215</v>
@@ -7544,7 +7701,7 @@
     </row>
     <row r="134" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>216</v>
@@ -7577,7 +7734,7 @@
     </row>
     <row r="135" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B135" s="19" t="s">
         <v>217</v>
@@ -7610,7 +7767,7 @@
     </row>
     <row r="136" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B136" s="19" t="s">
         <v>218</v>
@@ -7643,7 +7800,7 @@
     </row>
     <row r="137" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B137" s="19" t="s">
         <v>219</v>
@@ -7676,7 +7833,7 @@
     </row>
     <row r="138" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>220</v>
@@ -7709,7 +7866,7 @@
     </row>
     <row r="139" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B139" s="31" t="s">
         <v>221</v>
@@ -7742,7 +7899,7 @@
     </row>
     <row r="140" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B140" s="33" t="s">
         <v>222</v>
@@ -7775,7 +7932,7 @@
     </row>
     <row r="141" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B141" s="33" t="s">
         <v>223</v>
@@ -7808,7 +7965,7 @@
     </row>
     <row r="142" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B142" s="11" t="s">
         <v>224</v>
@@ -7840,7 +7997,7 @@
     </row>
     <row r="143" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>225</v>
@@ -7873,7 +8030,7 @@
     </row>
     <row r="144" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>226</v>
@@ -7906,7 +8063,7 @@
     </row>
     <row r="145" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>227</v>
@@ -7936,7 +8093,7 @@
     </row>
     <row r="146" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>228</v>
@@ -7966,7 +8123,7 @@
     </row>
     <row r="147" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>229</v>
@@ -7999,7 +8156,7 @@
     </row>
     <row r="148" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>230</v>
@@ -8032,7 +8189,7 @@
     </row>
     <row r="149" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>231</v>
@@ -8065,7 +8222,7 @@
     </row>
     <row r="150" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>232</v>
@@ -8095,7 +8252,7 @@
     </row>
     <row r="151" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>233</v>
@@ -8375,12 +8532,12 @@
         <v>248</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>251</v>
+        <v>421</v>
       </c>
       <c r="C160" s="32" t="s">
         <v>22</v>
@@ -8407,12 +8564,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A161" s="39" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>253</v>
+        <v>422</v>
       </c>
       <c r="C161" t="s">
         <v>22</v>
@@ -8435,15 +8592,15 @@
         <v>26</v>
       </c>
       <c r="L161" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A162" s="39" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C162" t="s">
         <v>22</v>
@@ -8466,15 +8623,15 @@
         <v>26</v>
       </c>
       <c r="L162" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A163" s="39" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="163" spans="1:12" ht="24" x14ac:dyDescent="0.2">
-      <c r="A163" s="39" t="s">
-        <v>256</v>
-      </c>
       <c r="B163" s="2" t="s">
-        <v>257</v>
+        <v>423</v>
       </c>
       <c r="C163" t="s">
         <v>22</v>
@@ -8497,15 +8654,15 @@
         <v>26</v>
       </c>
       <c r="L163" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="164" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A164" s="39" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>259</v>
+        <v>424</v>
       </c>
       <c r="C164" t="s">
         <v>22</v>
@@ -8528,15 +8685,15 @@
         <v>26</v>
       </c>
       <c r="L164" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A165" s="39" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C165" t="s">
         <v>22</v>
@@ -8559,15 +8716,15 @@
         <v>26</v>
       </c>
       <c r="L165" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A166" s="39" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C166" t="s">
         <v>22</v>
@@ -8590,15 +8747,15 @@
         <v>26</v>
       </c>
       <c r="L166" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A167" s="39" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C167" t="s">
         <v>22</v>
@@ -8621,15 +8778,15 @@
         <v>26</v>
       </c>
       <c r="L167" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="168" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A168" s="39" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C168" t="s">
         <v>22</v>
@@ -8652,15 +8809,15 @@
         <v>26</v>
       </c>
       <c r="L168" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A169" s="39" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C169" t="s">
         <v>22</v>
@@ -8683,15 +8840,15 @@
         <v>26</v>
       </c>
       <c r="L169" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A170" s="39" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C170" t="s">
         <v>22</v>
@@ -8714,15 +8871,15 @@
         <v>26</v>
       </c>
       <c r="L170" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="171" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A171" s="39" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C171" t="s">
         <v>22</v>
@@ -8745,15 +8902,15 @@
         <v>26</v>
       </c>
       <c r="L171" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A172" s="39" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C172" t="s">
         <v>59</v>
@@ -8776,15 +8933,15 @@
         <v>17</v>
       </c>
       <c r="L172" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A173" s="39" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C173" t="s">
         <v>22</v>
@@ -8807,15 +8964,15 @@
         <v>26</v>
       </c>
       <c r="L173" s="39" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="174" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A174" s="39" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C174" t="s">
         <v>22</v>
@@ -8838,15 +8995,15 @@
         <v>26</v>
       </c>
       <c r="L174" s="39" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="175" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A175" s="39" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C175" t="s">
         <v>22</v>
@@ -8869,15 +9026,15 @@
         <v>26</v>
       </c>
       <c r="L175" s="39" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="176" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A176" s="39" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C176" t="s">
         <v>22</v>
@@ -8900,15 +9057,15 @@
         <v>26</v>
       </c>
       <c r="L176" s="39" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A177" s="39" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C177" t="s">
         <v>22</v>
@@ -8931,15 +9088,15 @@
         <v>17</v>
       </c>
       <c r="L177" s="39" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A178" s="39" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C178" t="s">
         <v>22</v>
@@ -8962,15 +9119,15 @@
         <v>17</v>
       </c>
       <c r="L178" s="39" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A179" s="39" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C179" t="s">
         <v>22</v>
@@ -8993,15 +9150,15 @@
         <v>26</v>
       </c>
       <c r="L179" s="39" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A180" s="39" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C180" t="s">
         <v>22</v>
@@ -9024,15 +9181,15 @@
         <v>17</v>
       </c>
       <c r="L180" s="39" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A181" s="39" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C181" t="s">
         <v>22</v>
@@ -9055,15 +9212,15 @@
         <v>17</v>
       </c>
       <c r="L181" s="39" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A182" s="39" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C182" t="s">
         <v>59</v>
@@ -9092,10 +9249,10 @@
     </row>
     <row r="183" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A183" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="C183" t="s">
         <v>59</v>
@@ -9124,10 +9281,10 @@
     </row>
     <row r="184" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A184" s="39" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C184" t="s">
         <v>59</v>
@@ -9156,10 +9313,10 @@
     </row>
     <row r="185" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A185" s="39" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C185" t="s">
         <v>59</v>
@@ -9188,10 +9345,10 @@
     </row>
     <row r="186" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A186" s="39" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C186" t="s">
         <v>59</v>
@@ -9220,10 +9377,10 @@
     </row>
     <row r="187" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A187" s="39" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C187" t="s">
         <v>59</v>
@@ -9246,210 +9403,552 @@
         <v>17</v>
       </c>
       <c r="L187" s="39" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A188" s="39" t="s">
+        <v>405</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C188" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188" t="s">
+        <v>83</v>
+      </c>
+      <c r="E188"/>
+      <c r="F188" t="s">
+        <v>24</v>
+      </c>
+      <c r="G188" t="s">
+        <v>28</v>
+      </c>
+      <c r="H188" t="s">
+        <v>26</v>
+      </c>
+      <c r="I188"/>
+      <c r="K188" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A189" s="39" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A188" s="39"/>
-      <c r="C188"/>
-      <c r="D188"/>
-      <c r="E188"/>
-      <c r="F188"/>
-      <c r="G188"/>
-      <c r="H188"/>
-      <c r="I188"/>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A189" s="39"/>
-      <c r="C189"/>
-      <c r="D189"/>
+      <c r="B189" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C189" t="s">
+        <v>22</v>
+      </c>
+      <c r="D189" t="s">
+        <v>83</v>
+      </c>
       <c r="E189"/>
-      <c r="F189"/>
-      <c r="G189"/>
-      <c r="H189"/>
+      <c r="F189" t="s">
+        <v>24</v>
+      </c>
+      <c r="G189" t="s">
+        <v>28</v>
+      </c>
+      <c r="H189" t="s">
+        <v>26</v>
+      </c>
       <c r="I189"/>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A190" s="39"/>
-      <c r="C190"/>
-      <c r="D190"/>
+      <c r="K189" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+      <c r="A190" s="39" t="s">
+        <v>407</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C190" t="s">
+        <v>22</v>
+      </c>
+      <c r="D190" t="s">
+        <v>83</v>
+      </c>
       <c r="E190"/>
-      <c r="F190"/>
-      <c r="G190"/>
-      <c r="H190"/>
+      <c r="F190" t="s">
+        <v>24</v>
+      </c>
+      <c r="G190" t="s">
+        <v>28</v>
+      </c>
+      <c r="H190" t="s">
+        <v>26</v>
+      </c>
       <c r="I190"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A191" s="39"/>
-      <c r="C191"/>
-      <c r="D191"/>
+      <c r="K190" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" ht="36" x14ac:dyDescent="0.2">
+      <c r="A191" s="39" t="s">
+        <v>408</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C191" t="s">
+        <v>22</v>
+      </c>
+      <c r="D191" t="s">
+        <v>83</v>
+      </c>
       <c r="E191"/>
-      <c r="F191"/>
-      <c r="G191"/>
-      <c r="H191"/>
+      <c r="F191" t="s">
+        <v>24</v>
+      </c>
+      <c r="G191" t="s">
+        <v>28</v>
+      </c>
+      <c r="H191" t="s">
+        <v>26</v>
+      </c>
       <c r="I191"/>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A192" s="39"/>
-      <c r="C192"/>
-      <c r="D192"/>
+      <c r="K191" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" ht="84" x14ac:dyDescent="0.2">
+      <c r="A192" s="39" t="s">
+        <v>416</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C192" t="s">
+        <v>22</v>
+      </c>
+      <c r="D192" t="s">
+        <v>83</v>
+      </c>
       <c r="E192"/>
-      <c r="F192"/>
-      <c r="G192"/>
-      <c r="H192"/>
+      <c r="F192" t="s">
+        <v>24</v>
+      </c>
+      <c r="G192" t="s">
+        <v>28</v>
+      </c>
+      <c r="H192" t="s">
+        <v>17</v>
+      </c>
       <c r="I192"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A193" s="39"/>
-      <c r="C193"/>
-      <c r="D193"/>
+    <row r="193" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A193" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C193" t="s">
+        <v>22</v>
+      </c>
+      <c r="D193" t="s">
+        <v>83</v>
+      </c>
       <c r="E193"/>
-      <c r="F193"/>
-      <c r="G193"/>
-      <c r="H193"/>
+      <c r="F193" t="s">
+        <v>24</v>
+      </c>
+      <c r="G193" t="s">
+        <v>28</v>
+      </c>
+      <c r="H193" t="s">
+        <v>17</v>
+      </c>
       <c r="I193"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A194" s="39"/>
-      <c r="C194"/>
-      <c r="D194"/>
+    <row r="194" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A194" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C194" t="s">
+        <v>22</v>
+      </c>
+      <c r="D194" t="s">
+        <v>83</v>
+      </c>
       <c r="E194"/>
-      <c r="F194"/>
-      <c r="G194"/>
-      <c r="H194"/>
+      <c r="F194" t="s">
+        <v>24</v>
+      </c>
+      <c r="G194" t="s">
+        <v>28</v>
+      </c>
+      <c r="H194" t="s">
+        <v>26</v>
+      </c>
       <c r="I194"/>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A195" s="39"/>
-      <c r="C195"/>
-      <c r="D195"/>
+      <c r="K194" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A195" s="39" t="s">
+        <v>410</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C195" t="s">
+        <v>22</v>
+      </c>
+      <c r="D195" t="s">
+        <v>83</v>
+      </c>
       <c r="E195"/>
-      <c r="F195"/>
-      <c r="G195"/>
-      <c r="H195"/>
+      <c r="F195" t="s">
+        <v>24</v>
+      </c>
+      <c r="G195" t="s">
+        <v>28</v>
+      </c>
+      <c r="H195" t="s">
+        <v>26</v>
+      </c>
       <c r="I195"/>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A196" s="39"/>
-      <c r="C196"/>
-      <c r="D196"/>
+      <c r="K195" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" ht="108" x14ac:dyDescent="0.2">
+      <c r="A196" s="39" t="s">
+        <v>419</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C196" t="s">
+        <v>22</v>
+      </c>
+      <c r="D196" t="s">
+        <v>83</v>
+      </c>
       <c r="E196"/>
-      <c r="F196"/>
-      <c r="G196"/>
-      <c r="H196"/>
+      <c r="F196" t="s">
+        <v>24</v>
+      </c>
+      <c r="G196" t="s">
+        <v>28</v>
+      </c>
+      <c r="H196" t="s">
+        <v>17</v>
+      </c>
       <c r="I196"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A197" s="39"/>
-      <c r="C197"/>
-      <c r="D197"/>
+    <row r="197" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A197" s="39" t="s">
+        <v>420</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C197" t="s">
+        <v>22</v>
+      </c>
+      <c r="D197" t="s">
+        <v>83</v>
+      </c>
       <c r="E197"/>
-      <c r="F197"/>
-      <c r="G197"/>
-      <c r="H197"/>
+      <c r="F197" t="s">
+        <v>24</v>
+      </c>
+      <c r="G197" t="s">
+        <v>28</v>
+      </c>
+      <c r="H197" t="s">
+        <v>17</v>
+      </c>
       <c r="I197"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A198" s="39"/>
-      <c r="C198"/>
-      <c r="D198"/>
+    <row r="198" spans="1:11" ht="33" x14ac:dyDescent="0.2">
+      <c r="A198" s="39" t="s">
+        <v>425</v>
+      </c>
+      <c r="B198" s="42" t="s">
+        <v>426</v>
+      </c>
+      <c r="C198" t="s">
+        <v>22</v>
+      </c>
+      <c r="D198" t="s">
+        <v>148</v>
+      </c>
       <c r="E198"/>
-      <c r="F198"/>
-      <c r="G198"/>
-      <c r="H198"/>
+      <c r="F198" t="s">
+        <v>24</v>
+      </c>
+      <c r="G198" t="s">
+        <v>28</v>
+      </c>
+      <c r="H198" t="s">
+        <v>26</v>
+      </c>
       <c r="I198"/>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A199" s="39"/>
-      <c r="C199"/>
-      <c r="D199"/>
+      <c r="K198" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A199" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C199" t="s">
+        <v>59</v>
+      </c>
+      <c r="D199" t="s">
+        <v>431</v>
+      </c>
       <c r="E199"/>
-      <c r="F199"/>
-      <c r="G199"/>
-      <c r="H199"/>
+      <c r="F199" t="s">
+        <v>24</v>
+      </c>
+      <c r="G199" t="s">
+        <v>28</v>
+      </c>
+      <c r="H199" t="s">
+        <v>26</v>
+      </c>
       <c r="I199"/>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A200" s="39"/>
-      <c r="C200"/>
-      <c r="D200"/>
+      <c r="K199" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A200" s="39" t="s">
+        <v>428</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C200" t="s">
+        <v>59</v>
+      </c>
+      <c r="D200" t="s">
+        <v>431</v>
+      </c>
       <c r="E200"/>
-      <c r="F200"/>
-      <c r="G200"/>
-      <c r="H200"/>
+      <c r="F200" t="s">
+        <v>24</v>
+      </c>
+      <c r="G200" t="s">
+        <v>28</v>
+      </c>
+      <c r="H200" t="s">
+        <v>26</v>
+      </c>
       <c r="I200"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A201" s="39"/>
-      <c r="C201"/>
-      <c r="D201"/>
+      <c r="K200" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A201" s="39" t="s">
+        <v>432</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C201" t="s">
+        <v>59</v>
+      </c>
+      <c r="D201" t="s">
+        <v>442</v>
+      </c>
       <c r="E201"/>
-      <c r="F201"/>
-      <c r="G201"/>
-      <c r="H201"/>
+      <c r="F201" t="s">
+        <v>24</v>
+      </c>
+      <c r="G201" t="s">
+        <v>28</v>
+      </c>
+      <c r="H201" t="s">
+        <v>26</v>
+      </c>
       <c r="I201"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A202" s="39"/>
-      <c r="C202"/>
-      <c r="D202"/>
+      <c r="K201" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A202" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="C202" t="s">
+        <v>59</v>
+      </c>
+      <c r="D202" t="s">
+        <v>442</v>
+      </c>
       <c r="E202"/>
-      <c r="F202"/>
-      <c r="G202"/>
-      <c r="H202"/>
+      <c r="F202" t="s">
+        <v>24</v>
+      </c>
+      <c r="G202" t="s">
+        <v>28</v>
+      </c>
+      <c r="H202" t="s">
+        <v>26</v>
+      </c>
       <c r="I202"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A203" s="39"/>
-      <c r="C203"/>
-      <c r="D203"/>
+      <c r="K202" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A203" s="39" t="s">
+        <v>434</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C203" t="s">
+        <v>59</v>
+      </c>
+      <c r="D203" t="s">
+        <v>442</v>
+      </c>
       <c r="E203"/>
-      <c r="F203"/>
-      <c r="G203"/>
-      <c r="H203"/>
+      <c r="F203" t="s">
+        <v>24</v>
+      </c>
+      <c r="G203" t="s">
+        <v>28</v>
+      </c>
+      <c r="H203" t="s">
+        <v>26</v>
+      </c>
       <c r="I203"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A204" s="39"/>
-      <c r="C204"/>
-      <c r="D204"/>
+      <c r="K203" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A204" s="39" t="s">
+        <v>435</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C204" t="s">
+        <v>59</v>
+      </c>
+      <c r="D204" t="s">
+        <v>442</v>
+      </c>
       <c r="E204"/>
-      <c r="F204"/>
-      <c r="G204"/>
-      <c r="H204"/>
+      <c r="F204" t="s">
+        <v>24</v>
+      </c>
+      <c r="G204" t="s">
+        <v>28</v>
+      </c>
+      <c r="H204" t="s">
+        <v>26</v>
+      </c>
       <c r="I204"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A205" s="39"/>
-      <c r="C205"/>
-      <c r="D205"/>
+      <c r="K204" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A205" s="39" t="s">
+        <v>436</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C205" t="s">
+        <v>59</v>
+      </c>
+      <c r="D205" t="s">
+        <v>442</v>
+      </c>
       <c r="E205"/>
-      <c r="F205"/>
-      <c r="G205"/>
-      <c r="H205"/>
+      <c r="F205" t="s">
+        <v>24</v>
+      </c>
+      <c r="G205" t="s">
+        <v>28</v>
+      </c>
+      <c r="H205" t="s">
+        <v>26</v>
+      </c>
       <c r="I205"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A206" s="39"/>
-      <c r="C206"/>
-      <c r="D206"/>
+      <c r="K205" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A206" s="43" t="s">
+        <v>443</v>
+      </c>
+      <c r="B206" s="43" t="s">
+        <v>443</v>
+      </c>
+      <c r="C206" t="s">
+        <v>59</v>
+      </c>
+      <c r="D206" t="s">
+        <v>442</v>
+      </c>
       <c r="E206"/>
-      <c r="F206"/>
-      <c r="G206"/>
-      <c r="H206"/>
+      <c r="F206" t="s">
+        <v>24</v>
+      </c>
+      <c r="G206" t="s">
+        <v>28</v>
+      </c>
+      <c r="H206" t="s">
+        <v>17</v>
+      </c>
       <c r="I206"/>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A207" s="39"/>
-      <c r="C207"/>
-      <c r="D207"/>
+    <row r="207" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="A207" s="39" t="s">
+        <v>444</v>
+      </c>
+      <c r="B207" s="39" t="s">
+        <v>444</v>
+      </c>
+      <c r="C207" t="s">
+        <v>59</v>
+      </c>
+      <c r="D207" t="s">
+        <v>442</v>
+      </c>
       <c r="E207"/>
-      <c r="F207"/>
-      <c r="G207"/>
-      <c r="H207"/>
+      <c r="F207" t="s">
+        <v>24</v>
+      </c>
+      <c r="G207" t="s">
+        <v>28</v>
+      </c>
+      <c r="H207" t="s">
+        <v>17</v>
+      </c>
       <c r="I207"/>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" s="39"/>
       <c r="C208"/>
       <c r="D208"/>
@@ -12369,53 +12868,79 @@
       <c r="H499"/>
       <c r="I499"/>
     </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A500" s="39"/>
+      <c r="C500"/>
+      <c r="D500"/>
+      <c r="E500"/>
+      <c r="F500"/>
+      <c r="G500"/>
+      <c r="H500"/>
+      <c r="I500"/>
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A501" s="39"/>
+      <c r="C501"/>
+      <c r="D501"/>
+      <c r="E501"/>
+      <c r="F501"/>
+      <c r="G501"/>
+      <c r="H501"/>
+      <c r="I501"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:M197" xr:uid="{E474665A-CDEB-4757-8FC6-0AC249C250E7}"/>
   <conditionalFormatting sqref="M1:IN1">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="65">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="66">
       <formula>LEN(TRIM(M1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A182:E186 I182:IO186 A187:IO1048576">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="64">
+  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A182:E186 I182:IO186 A187:IO197 A198 C198:IO198 A199:IO200 C206:E206 A202:E205 F202:F206 A201:F201 A208:IO1048576 A207:B207 I207:IO207 G201:IO206">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="65">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122:H122">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="63" priority="43">
       <formula>LEN(TRIM(B122))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M92:IO107">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="63">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="64">
       <formula>LEN(TRIM(M92))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126:H126">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="39">
       <formula>LEN(TRIM(B126))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B127:H127">
-    <cfRule type="notContainsBlanks" dxfId="59" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="38">
       <formula>LEN(TRIM(B127))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K161:K172 K182:K1048576">
-    <cfRule type="containsText" dxfId="58" priority="61" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="58" priority="63" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:J141">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="34">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="35">
       <formula>LEN(TRIM(B140))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K140:K141">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="34">
       <formula>LEN(TRIM(K140))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B138:J139">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="31">
+      <formula>LEN(TRIM(B138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138:J139">
@@ -12423,42 +12948,42 @@
       <formula>LEN(TRIM(B138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B138:J139">
+  <conditionalFormatting sqref="K138:K139">
     <cfRule type="notContainsBlanks" dxfId="53" priority="29">
-      <formula>LEN(TRIM(B138))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K138:K139">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="28">
       <formula>LEN(TRIM(K138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:J143 L143">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="26">
       <formula>LEN(TRIM(B143))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K143">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="24">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="25">
       <formula>LEN(TRIM(K143))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:H147 J144:K147">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="22">
+      <formula>LEN(TRIM(C144))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C144:H147 J144:J147">
     <cfRule type="notContainsBlanks" dxfId="49" priority="21">
       <formula>LEN(TRIM(C144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C144:H147 J144:J147">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="20">
-      <formula>LEN(TRIM(C144))&gt;0</formula>
+  <conditionalFormatting sqref="K148:K151">
+    <cfRule type="containsText" dxfId="48" priority="10" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K148)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="11" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K148)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K148:K151">
-    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="No">
-      <formula>NOT(ISERROR(SEARCH("No",K148)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",K148)))</formula>
+  <conditionalFormatting sqref="I148:I151">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="13">
+      <formula>LEN(TRIM(I148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I151">
@@ -12466,79 +12991,79 @@
       <formula>LEN(TRIM(I148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I148:I151">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="11">
-      <formula>LEN(TRIM(I148))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:L1">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="60">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="61">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B117:J117">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="47">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="48">
       <formula>LEN(TRIM(B117))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B118:H118">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="47">
       <formula>LEN(TRIM(B118))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119:H119">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="45">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="46">
       <formula>LEN(TRIM(B119))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B120:H120">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="45">
       <formula>LEN(TRIM(B120))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:H121">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="44">
       <formula>LEN(TRIM(B121))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:H123">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="42">
       <formula>LEN(TRIM(B123))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L91">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
       <formula>LEN(TRIM(L91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:J141">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
       <formula>LEN(TRIM(B140))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B148:B151">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
       <formula>LEN(TRIM(B148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:J10 B2:J8 C9:D9 F9:H9 J9 B84:J98 B99:H99 J99 B100:J109 L2:L90 B11:B44 B110:K112 I113:K116 K117 B118:K118 I119:K127 L92:L142 B142:K142 B47:B62 B64:B83 C11:J83 K2:K109 B128:K137 B144:B147 L144:L155 B152:K155 A2:A155">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="59">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="60">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="58">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="59">
       <formula>LEN(TRIM(I9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:A101 B84:B99 C84:J98 C99:H99 J99 L92:L107">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="57">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="58">
       <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:A111 A113:A115">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="57">
+      <formula>LEN(TRIM(A110))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I99">
     <cfRule type="notContainsBlanks" dxfId="30" priority="56">
-      <formula>LEN(TRIM(A110))&gt;0</formula>
+      <formula>LEN(TRIM(I99))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I99">
@@ -12546,71 +13071,71 @@
       <formula>LEN(TRIM(I99))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I99">
-    <cfRule type="notContainsBlanks" dxfId="28" priority="54">
-      <formula>LEN(TRIM(I99))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K142 K152:K155 K2:K137">
-    <cfRule type="containsText" dxfId="27" priority="52" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="28" priority="53" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="53" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="54" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113:H113">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="51">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="52">
       <formula>LEN(TRIM(B113))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114:H114">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="50">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="51">
       <formula>LEN(TRIM(B114))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115:H115">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="49">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="50">
       <formula>LEN(TRIM(B115))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116:H116">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="48">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="49">
       <formula>LEN(TRIM(B116))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124:H124">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="41">
       <formula>LEN(TRIM(B124))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125:H125">
-    <cfRule type="notContainsBlanks" dxfId="20" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="40">
       <formula>LEN(TRIM(B125))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K138:K139">
-    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K140:K141">
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="18" priority="32" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K140)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K143">
-    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K143)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I144:I147">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="20">
+      <formula>LEN(TRIM(I144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I144:I147">
@@ -12618,68 +13143,71 @@
       <formula>LEN(TRIM(I144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I144:I147">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="18">
-      <formula>LEN(TRIM(I144))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K144:K147">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C148:H151 J148:K151">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
+      <formula>LEN(TRIM(C148))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C148:H151 J148:J151">
     <cfRule type="notContainsBlanks" dxfId="9" priority="14">
       <formula>LEN(TRIM(C148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C148:H151 J148:J151">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
-      <formula>LEN(TRIM(C148))&gt;0</formula>
+  <conditionalFormatting sqref="L156:L160 A156:J160">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(A156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L156:L160 A156:J160">
+  <conditionalFormatting sqref="A156 A158:A160">
     <cfRule type="notContainsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(A156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A156 A158:A160">
+  <conditionalFormatting sqref="K156:K160">
     <cfRule type="notContainsBlanks" dxfId="6" priority="7">
-      <formula>LEN(TRIM(A156))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K156:K160">
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(K156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K156:K160">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173:IO173 A174:L181 F182:H186">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(A173))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K173:K181">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K173)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K173)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Wrong values" error="The cell accepts only Yes/No values." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <conditionalFormatting sqref="C207:H207">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(C207))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Wrong values" error="The cell accepts only Yes/No values." sqref="K2:K201 K203:K204 K206:K1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Wrong values" error="The cell accepts only Yes/No values." sqref="K205 K202" xr:uid="{F8F85F5E-7CB4-430B-8002-6B25041180E0}">
+      <formula1>"Yes,No,FINSUS2,FINSUS5"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12688,21 +13216,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D8B37618F89864ABE738DE1DBF7EE19" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4c6f3c0ade2d5a986931f6ef6dfeb08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1543e12e-b41e-4b3f-8a83-41e12152c6a2" xmlns:ns3="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e00bb17d7a9f5ad1136a799a86145782" ns2:_="" ns3:_="">
     <xsd:import namespace="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
@@ -12905,32 +13418,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
-    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C46AAE6-A078-49FB-B5E7-EEC8BF2D1038}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12947,4 +13450,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
+    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update with 20-21 data
</commit_message>
<xml_diff>
--- a/data/Metadata - Shiny.xlsx
+++ b/data/Metadata - Shiny.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\OneDrive - IS\LGBF-Spotfire\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassidy.nicholas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C92578-C1B8-4CDD-89B5-AC348BD92276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B2EBA9C-BA4A-4FA8-ADAF-81B80D7FA786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="453">
   <si>
     <t>Variable name</t>
   </si>
@@ -1372,6 +1372,30 @@
   </si>
   <si>
     <t xml:space="preserve">Net budgeted revenue expenditure as reported to committee (£000s) </t>
+  </si>
+  <si>
+    <t>CHN24</t>
+  </si>
+  <si>
+    <t>Percentage of children living in poverty (after housing costs)</t>
+  </si>
+  <si>
+    <t>ECON11</t>
+  </si>
+  <si>
+    <t>ECON12a</t>
+  </si>
+  <si>
+    <t>ECON12b</t>
+  </si>
+  <si>
+    <t>Gross Value Added (GVA) per capita</t>
+  </si>
+  <si>
+    <t>Claimant Count as a percentage of Working Age Population</t>
+  </si>
+  <si>
+    <t>Claimant Count as a percentage of 16-24 Population</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1732,207 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="82">
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="hair">
@@ -3033,8 +3257,8 @@
   <dimension ref="A1:IN501"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K205" sqref="K205"/>
+      <pane ySplit="1" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D219" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -9543,7 +9767,7 @@
       </c>
       <c r="I192"/>
     </row>
-    <row r="193" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A193" s="39" t="s">
         <v>417</v>
       </c>
@@ -9568,7 +9792,7 @@
       </c>
       <c r="I193"/>
     </row>
-    <row r="194" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A194" s="39" t="s">
         <v>409</v>
       </c>
@@ -9596,7 +9820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A195" s="39" t="s">
         <v>410</v>
       </c>
@@ -9624,7 +9848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="108" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12" ht="108" x14ac:dyDescent="0.2">
       <c r="A196" s="39" t="s">
         <v>419</v>
       </c>
@@ -9649,7 +9873,7 @@
       </c>
       <c r="I196"/>
     </row>
-    <row r="197" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A197" s="39" t="s">
         <v>420</v>
       </c>
@@ -9674,7 +9898,7 @@
       </c>
       <c r="I197"/>
     </row>
-    <row r="198" spans="1:11" ht="33" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12" ht="33" x14ac:dyDescent="0.2">
       <c r="A198" s="39" t="s">
         <v>425</v>
       </c>
@@ -9702,7 +9926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A199" s="39" t="s">
         <v>427</v>
       </c>
@@ -9730,7 +9954,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A200" s="39" t="s">
         <v>428</v>
       </c>
@@ -9758,7 +9982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A201" s="39" t="s">
         <v>432</v>
       </c>
@@ -9786,7 +10010,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A202" s="39" t="s">
         <v>433</v>
       </c>
@@ -9814,7 +10038,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A203" s="39" t="s">
         <v>434</v>
       </c>
@@ -9842,7 +10066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12" ht="36" x14ac:dyDescent="0.2">
       <c r="A204" s="39" t="s">
         <v>435</v>
       </c>
@@ -9870,7 +10094,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12" ht="24" x14ac:dyDescent="0.2">
       <c r="A205" s="39" t="s">
         <v>436</v>
       </c>
@@ -9898,7 +10122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A206" s="43" t="s">
         <v>443</v>
       </c>
@@ -9923,7 +10147,7 @@
       </c>
       <c r="I206"/>
     </row>
-    <row r="207" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12" ht="96" x14ac:dyDescent="0.2">
       <c r="A207" s="39" t="s">
         <v>444</v>
       </c>
@@ -9948,47 +10172,134 @@
       </c>
       <c r="I207"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A208" s="39"/>
-      <c r="C208"/>
-      <c r="D208"/>
+    <row r="208" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="A208" s="39" t="s">
+        <v>445</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C208" t="s">
+        <v>22</v>
+      </c>
+      <c r="D208" t="s">
+        <v>23</v>
+      </c>
       <c r="E208"/>
-      <c r="F208"/>
-      <c r="G208"/>
-      <c r="H208"/>
+      <c r="F208" t="s">
+        <v>24</v>
+      </c>
+      <c r="G208" t="s">
+        <v>28</v>
+      </c>
+      <c r="H208" t="s">
+        <v>26</v>
+      </c>
       <c r="I208"/>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A209" s="39"/>
-      <c r="C209"/>
-      <c r="D209"/>
+      <c r="K208" t="s">
+        <v>17</v>
+      </c>
+      <c r="L208" s="39" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="A209" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C209" t="s">
+        <v>59</v>
+      </c>
+      <c r="D209" t="s">
+        <v>170</v>
+      </c>
       <c r="E209"/>
-      <c r="F209"/>
-      <c r="G209"/>
-      <c r="H209"/>
+      <c r="F209" t="s">
+        <v>24</v>
+      </c>
+      <c r="G209" t="s">
+        <v>28</v>
+      </c>
+      <c r="H209" t="s">
+        <v>26</v>
+      </c>
       <c r="I209"/>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A210" s="39"/>
-      <c r="C210"/>
-      <c r="D210"/>
+      <c r="K209" t="s">
+        <v>26</v>
+      </c>
+      <c r="L209" t="str">
+        <f t="shared" ref="L209" si="4">A209</f>
+        <v>ECON11</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="A210" s="39" t="s">
+        <v>448</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C210" t="s">
+        <v>59</v>
+      </c>
+      <c r="D210" t="s">
+        <v>170</v>
+      </c>
       <c r="E210"/>
-      <c r="F210"/>
-      <c r="G210"/>
-      <c r="H210"/>
+      <c r="F210" t="s">
+        <v>24</v>
+      </c>
+      <c r="G210" t="s">
+        <v>28</v>
+      </c>
+      <c r="H210" t="s">
+        <v>26</v>
+      </c>
       <c r="I210"/>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A211" s="39"/>
-      <c r="C211"/>
-      <c r="D211"/>
+      <c r="K210" t="s">
+        <v>17</v>
+      </c>
+      <c r="L210" t="str">
+        <f t="shared" ref="L210:L211" si="5">A210</f>
+        <v>ECON12a</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+      <c r="A211" s="39" t="s">
+        <v>449</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C211" t="s">
+        <v>59</v>
+      </c>
+      <c r="D211" t="s">
+        <v>170</v>
+      </c>
       <c r="E211"/>
-      <c r="F211"/>
-      <c r="G211"/>
-      <c r="H211"/>
+      <c r="F211" t="s">
+        <v>24</v>
+      </c>
+      <c r="G211" t="s">
+        <v>28</v>
+      </c>
+      <c r="H211" t="s">
+        <v>26</v>
+      </c>
       <c r="I211"/>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K211" t="s">
+        <v>17</v>
+      </c>
+      <c r="L211" t="str">
+        <f t="shared" si="5"/>
+        <v>ECON12b</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" s="39"/>
       <c r="C212"/>
       <c r="D212"/>
@@ -9998,7 +10309,7 @@
       <c r="H212"/>
       <c r="I212"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" s="39"/>
       <c r="C213"/>
       <c r="D213"/>
@@ -10008,7 +10319,7 @@
       <c r="H213"/>
       <c r="I213"/>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A214" s="39"/>
       <c r="C214"/>
       <c r="D214"/>
@@ -10018,7 +10329,7 @@
       <c r="H214"/>
       <c r="I214"/>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A215" s="39"/>
       <c r="C215"/>
       <c r="D215"/>
@@ -10028,7 +10339,7 @@
       <c r="H215"/>
       <c r="I215"/>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" s="39"/>
       <c r="C216"/>
       <c r="D216"/>
@@ -10038,7 +10349,7 @@
       <c r="H216"/>
       <c r="I216"/>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" s="39"/>
       <c r="C217"/>
       <c r="D217"/>
@@ -10048,7 +10359,7 @@
       <c r="H217"/>
       <c r="I217"/>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" s="39"/>
       <c r="C218"/>
       <c r="D218"/>
@@ -10058,7 +10369,7 @@
       <c r="H218"/>
       <c r="I218"/>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A219" s="39"/>
       <c r="C219"/>
       <c r="D219"/>
@@ -10068,7 +10379,7 @@
       <c r="H219"/>
       <c r="I219"/>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" s="39"/>
       <c r="C220"/>
       <c r="D220"/>
@@ -10078,7 +10389,7 @@
       <c r="H220"/>
       <c r="I220"/>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" s="39"/>
       <c r="C221"/>
       <c r="D221"/>
@@ -10088,7 +10399,7 @@
       <c r="H221"/>
       <c r="I221"/>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" s="39"/>
       <c r="C222"/>
       <c r="D222"/>
@@ -10098,7 +10409,7 @@
       <c r="H222"/>
       <c r="I222"/>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" s="39"/>
       <c r="C223"/>
       <c r="D223"/>
@@ -10108,7 +10419,7 @@
       <c r="H223"/>
       <c r="I223"/>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A224" s="39"/>
       <c r="C224"/>
       <c r="D224"/>
@@ -12891,315 +13202,387 @@
   </sheetData>
   <autoFilter ref="A1:M197" xr:uid="{E474665A-CDEB-4757-8FC6-0AC249C250E7}"/>
   <conditionalFormatting sqref="M1:IN1">
-    <cfRule type="notContainsBlanks" dxfId="65" priority="66">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="82">
       <formula>LEN(TRIM(M1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A182:E186 I182:IO186 A187:IO197 A198 C198:IO198 A199:IO200 C206:E206 A202:E205 F202:F206 A201:F201 A208:IO1048576 A207:B207 I207:IO207 G201:IO206">
-    <cfRule type="notContainsBlanks" dxfId="64" priority="65">
+  <conditionalFormatting sqref="M2:IO172 A161:L172 M174:IO181 A182:E186 I182:IO186 A187:IO197 A198 C198:IO198 A199:IO200 C206:E206 A202:E205 F202:F206 A201:F201 A212:IO1048576 A207:B207 I207:IO207 G201:IO206">
+    <cfRule type="notContainsBlanks" dxfId="80" priority="81">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122:H122">
-    <cfRule type="notContainsBlanks" dxfId="63" priority="43">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="59">
       <formula>LEN(TRIM(B122))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M92:IO107">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="64">
+    <cfRule type="notContainsBlanks" dxfId="78" priority="80">
       <formula>LEN(TRIM(M92))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126:H126">
-    <cfRule type="notContainsBlanks" dxfId="61" priority="39">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="55">
       <formula>LEN(TRIM(B126))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B127:H127">
-    <cfRule type="notContainsBlanks" dxfId="60" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="76" priority="54">
       <formula>LEN(TRIM(B127))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K161:K172 K182:K1048576">
-    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="No">
+  <conditionalFormatting sqref="K161:K172 K182:K207 K212:K1048576">
+    <cfRule type="containsText" dxfId="75" priority="78" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K161)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="63" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="79" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K161)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:J141">
-    <cfRule type="notContainsBlanks" dxfId="57" priority="35">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="51">
       <formula>LEN(TRIM(B140))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K140:K141">
-    <cfRule type="notContainsBlanks" dxfId="56" priority="34">
+    <cfRule type="notContainsBlanks" dxfId="72" priority="50">
       <formula>LEN(TRIM(K140))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138:J139">
-    <cfRule type="notContainsBlanks" dxfId="55" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="47">
       <formula>LEN(TRIM(B138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138:J139">
-    <cfRule type="notContainsBlanks" dxfId="54" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="70" priority="46">
       <formula>LEN(TRIM(B138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K138:K139">
-    <cfRule type="notContainsBlanks" dxfId="53" priority="29">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="45">
       <formula>LEN(TRIM(K138))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:J143 L143">
-    <cfRule type="notContainsBlanks" dxfId="52" priority="26">
+    <cfRule type="notContainsBlanks" dxfId="68" priority="42">
       <formula>LEN(TRIM(B143))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K143">
-    <cfRule type="notContainsBlanks" dxfId="51" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="67" priority="41">
       <formula>LEN(TRIM(K143))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:H147 J144:K147">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="38">
       <formula>LEN(TRIM(C144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C144:H147 J144:J147">
-    <cfRule type="notContainsBlanks" dxfId="49" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="65" priority="37">
       <formula>LEN(TRIM(C144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K148:K151">
-    <cfRule type="containsText" dxfId="48" priority="10" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="26" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K148)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="11" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="63" priority="27" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K148)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I151">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="29">
       <formula>LEN(TRIM(I148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I148:I151">
-    <cfRule type="notContainsBlanks" dxfId="45" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="61" priority="28">
       <formula>LEN(TRIM(I148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:L1">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="61">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="77">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B117:J117">
-    <cfRule type="notContainsBlanks" dxfId="43" priority="48">
+    <cfRule type="notContainsBlanks" dxfId="59" priority="64">
       <formula>LEN(TRIM(B117))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B118:H118">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="47">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="63">
       <formula>LEN(TRIM(B118))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119:H119">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="62">
       <formula>LEN(TRIM(B119))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B120:H120">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="45">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="61">
       <formula>LEN(TRIM(B120))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:H121">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="44">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="60">
       <formula>LEN(TRIM(B121))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:H123">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="42">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="58">
       <formula>LEN(TRIM(B123))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L91">
-    <cfRule type="notContainsBlanks" dxfId="37" priority="37">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="53">
       <formula>LEN(TRIM(L91))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:J141">
-    <cfRule type="notContainsBlanks" dxfId="36" priority="36">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="52">
       <formula>LEN(TRIM(B140))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B148:B151">
-    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
+    <cfRule type="notContainsBlanks" dxfId="51" priority="32">
       <formula>LEN(TRIM(B148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:J10 B2:J8 C9:D9 F9:H9 J9 B84:J98 B99:H99 J99 B100:J109 L2:L90 B11:B44 B110:K112 I113:K116 K117 B118:K118 I119:K127 L92:L142 B142:K142 B47:B62 B64:B83 C11:J83 K2:K109 B128:K137 B144:B147 L144:L155 B152:K155 A2:A155">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="60">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="76">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="notContainsBlanks" dxfId="33" priority="59">
+    <cfRule type="notContainsBlanks" dxfId="49" priority="75">
       <formula>LEN(TRIM(I9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:A101 B84:B99 C84:J98 C99:H99 J99 L92:L107">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="58">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="74">
       <formula>LEN(TRIM(A84))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A110:A111 A113:A115">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="57">
+    <cfRule type="notContainsBlanks" dxfId="47" priority="73">
       <formula>LEN(TRIM(A110))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I99">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="56">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="72">
       <formula>LEN(TRIM(I99))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I99">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="55">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="71">
       <formula>LEN(TRIM(I99))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K142 K152:K155 K2:K137">
-    <cfRule type="containsText" dxfId="28" priority="53" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="44" priority="69" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="54" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="43" priority="70" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113:H113">
-    <cfRule type="notContainsBlanks" dxfId="26" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="68">
       <formula>LEN(TRIM(B113))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114:H114">
-    <cfRule type="notContainsBlanks" dxfId="25" priority="51">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="67">
       <formula>LEN(TRIM(B114))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115:H115">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="50">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="66">
       <formula>LEN(TRIM(B115))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B116:H116">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="49">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="65">
       <formula>LEN(TRIM(B116))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124:H124">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="41">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="57">
       <formula>LEN(TRIM(B124))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125:H125">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="56">
       <formula>LEN(TRIM(B125))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K138:K139">
-    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K138)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="35" priority="44" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K140:K141">
-    <cfRule type="containsText" dxfId="18" priority="32" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K140)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="33" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="33" priority="49" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K143">
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="32" priority="39" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K143)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="31" priority="40" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I144:I147">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="36">
       <formula>LEN(TRIM(I144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I144:I147">
-    <cfRule type="notContainsBlanks" dxfId="13" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="35">
       <formula>LEN(TRIM(I144))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K144:K147">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K144)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C148:H151 J148:K151">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="31">
       <formula>LEN(TRIM(C148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C148:H151 J148:J151">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="30">
       <formula>LEN(TRIM(C148))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L156:L160 A156:J160">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="25">
       <formula>LEN(TRIM(A156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A156 A158:A160">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24">
       <formula>LEN(TRIM(A156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K156:K160">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="23">
       <formula>LEN(TRIM(K156))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K156:K160">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K156)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K156)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A173:IO173 A174:L181 F182:H186">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="20">
       <formula>LEN(TRIM(A173))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K173:K181">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K173)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",K173)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C207:H207">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="17">
+      <formula>LEN(TRIM(C207))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M208:IO208">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(M208))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A208:L208">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(A208))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K208">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K208)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K208)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A209:E209 I209:IO209">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(A209))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K209">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K209)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K209)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F209:H209">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(F209))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A210:E210 I210:IO210">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(A210))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K210">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K210)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K210)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210:H210">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(F210))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A211:E211 I211:IO211">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(A211))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K211">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="No">
+      <formula>NOT(ISERROR(SEARCH("No",K211)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",K211)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F211:H211">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C207))&gt;0</formula>
+      <formula>LEN(TRIM(F211))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -13216,6 +13599,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D8B37618F89864ABE738DE1DBF7EE19" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4c6f3c0ade2d5a986931f6ef6dfeb08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1543e12e-b41e-4b3f-8a83-41e12152c6a2" xmlns:ns3="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e00bb17d7a9f5ad1136a799a86145782" ns2:_="" ns3:_="">
     <xsd:import namespace="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
@@ -13418,22 +13816,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
+    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C46AAE6-A078-49FB-B5E7-EEC8BF2D1038}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13450,29 +13858,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2748C6-A968-49EF-BF92-9B8E2B3269A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B15DCC0B-376D-4BDC-8CA6-8A07A59786FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1543e12e-b41e-4b3f-8a83-41e12152c6a2"/>
-    <ds:schemaRef ds:uri="4ea622ab-6d0b-4c8a-8736-27bd26b1fd54"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>